<commit_message>
error correction on imports / exports / total production
</commit_message>
<xml_diff>
--- a/scenario_data/scenario_data_excel.xlsx
+++ b/scenario_data/scenario_data_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joanna.schlesinger\0.Joanna\2. HySPI\RTE_scenarios\scenario_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C1A0D4-10BB-4B8B-888C-6D31DC89C1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4D7195-360C-4572-BEEC-F10FEF85C2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_data" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,12 +436,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -524,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -549,14 +543,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,13 +862,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA1387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E341" sqref="E341"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" customWidth="1"/>
     <col min="5" max="5" width="61.26953125" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" style="16" customWidth="1"/>
     <col min="12" max="12" width="11" style="16"/>
@@ -949,7 +943,7 @@
       <c r="U1" s="6">
         <v>2060</v>
       </c>
-      <c r="V1" s="19">
+      <c r="V1" s="16">
         <v>0.16</v>
       </c>
       <c r="W1" s="13" t="s">
@@ -1256,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1300,7 @@
         <v>101.5727651</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1356,7 +1350,7 @@
         <v>131.27276509999999</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1780,7 +1774,7 @@
         <f>(AA15-AA16)*$V1</f>
         <v>10.048</v>
       </c>
-      <c r="V15" s="24" t="s">
+      <c r="V15" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W15">
@@ -1870,7 +1864,7 @@
         <f>(AA15-AA16)*(1-$V1)</f>
         <v>52.752000000000002</v>
       </c>
-      <c r="V16" s="24" t="s">
+      <c r="V16" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W16">
@@ -2495,7 +2489,7 @@
       <c r="U25">
         <v>17.100000000000001</v>
       </c>
-      <c r="V25" s="20"/>
+      <c r="V25" s="19"/>
     </row>
     <row r="26" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -3060,7 +3054,7 @@
       <c r="D37" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="4" t="s">
         <v>48</v>
       </c>
       <c r="F37" t="s">
@@ -3110,7 +3104,7 @@
       <c r="D38" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F38" t="s">
@@ -3160,7 +3154,7 @@
       <c r="D39" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="4" t="s">
         <v>50</v>
       </c>
       <c r="F39" t="s">
@@ -3210,7 +3204,7 @@
       <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F40" t="s">
@@ -3260,7 +3254,7 @@
       <c r="D41" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F41" t="s">
@@ -3310,7 +3304,7 @@
       <c r="D42" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="25" t="s">
+      <c r="E42" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F42" t="s">
@@ -3360,7 +3354,7 @@
       <c r="D43" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="25" t="s">
+      <c r="E43" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F43" t="s">
@@ -3410,7 +3404,7 @@
       <c r="D44" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E44" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F44" t="s">
@@ -3460,7 +3454,7 @@
       <c r="D45" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="25" t="s">
+      <c r="E45" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F45" t="s">
@@ -3510,7 +3504,7 @@
       <c r="D46" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F46" t="s">
@@ -3560,7 +3554,7 @@
       <c r="D47" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="25" t="s">
+      <c r="E47" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F47" t="s">
@@ -3610,7 +3604,7 @@
       <c r="D48" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F48" t="s">
@@ -3660,7 +3654,7 @@
       <c r="D49" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="25" t="s">
+      <c r="E49" s="4" t="s">
         <v>60</v>
       </c>
       <c r="F49" t="s">
@@ -3710,7 +3704,7 @@
       <c r="D50" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="25" t="s">
+      <c r="E50" s="4" t="s">
         <v>61</v>
       </c>
       <c r="F50" t="s">
@@ -3760,7 +3754,7 @@
       <c r="D51" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="25" t="s">
+      <c r="E51" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F51" t="s">
@@ -3810,7 +3804,7 @@
       <c r="D52" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="25" t="s">
+      <c r="E52" s="4" t="s">
         <v>63</v>
       </c>
       <c r="F52" t="s">
@@ -3860,7 +3854,7 @@
       <c r="D53" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="4" t="s">
         <v>64</v>
       </c>
       <c r="F53" t="s">
@@ -3910,7 +3904,7 @@
       <c r="D54" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F54" t="s">
@@ -3960,7 +3954,7 @@
       <c r="D55" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F55" t="s">
@@ -4010,7 +4004,7 @@
       <c r="D56" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="25" t="s">
+      <c r="E56" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F56" t="s">
@@ -4060,7 +4054,7 @@
       <c r="D57" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="4" t="s">
         <v>68</v>
       </c>
       <c r="F57" t="s">
@@ -4110,7 +4104,7 @@
       <c r="D58" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="E58" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F58" t="s">
@@ -4160,7 +4154,7 @@
       <c r="D59" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="25" t="s">
+      <c r="E59" s="4" t="s">
         <v>70</v>
       </c>
       <c r="F59" t="s">
@@ -4210,7 +4204,7 @@
       <c r="D60" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="25" t="s">
+      <c r="E60" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F60" t="s">
@@ -4260,7 +4254,7 @@
       <c r="D61" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="25" t="s">
+      <c r="E61" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F61" t="s">
@@ -4310,7 +4304,7 @@
       <c r="D62" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="25" t="s">
+      <c r="E62" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F62" t="s">
@@ -4360,7 +4354,7 @@
       <c r="D63" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="25" t="s">
+      <c r="E63" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F63" t="s">
@@ -4997,7 +4991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -5047,7 +5041,7 @@
         <v>62.462262520000003</v>
       </c>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -5097,7 +5091,7 @@
         <v>97.062262520000004</v>
       </c>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -5521,7 +5515,7 @@
         <f>(AA83-AA84)*$V1</f>
         <v>10.048</v>
       </c>
-      <c r="V83" s="24" t="s">
+      <c r="V83" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W83">
@@ -5611,7 +5605,7 @@
         <f>(AA83-AA84)*(1-$V1)</f>
         <v>52.752000000000002</v>
       </c>
-      <c r="V84" s="24" t="s">
+      <c r="V84" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W84">
@@ -9261,7 +9255,7 @@
         <f>(AA151-AA152)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V151" s="24" t="s">
+      <c r="V151" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W151">
@@ -9351,7 +9345,7 @@
         <f>(AA151-AA152)*(1-$V1)</f>
         <v>52.667999999999992</v>
       </c>
-      <c r="V152" s="24" t="s">
+      <c r="V152" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W152">
@@ -13001,7 +12995,7 @@
         <f>(AA219-AA220)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V219" s="24" t="s">
+      <c r="V219" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W219">
@@ -13091,7 +13085,7 @@
         <f>(AA219-AA220)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V220" s="24" t="s">
+      <c r="V220" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W220">
@@ -16741,7 +16735,7 @@
         <f>(AA287-AA288)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V287" s="24" t="s">
+      <c r="V287" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W287">
@@ -16831,7 +16825,7 @@
         <f>(AA287-AA288)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V288" s="24" t="s">
+      <c r="V288" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W288">
@@ -18207,7 +18201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>6</v>
       </c>
@@ -18221,7 +18215,7 @@
         <v>9</v>
       </c>
       <c r="E313" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F313" t="s">
         <v>11</v>
@@ -18257,7 +18251,7 @@
         <v>39.444626509999999</v>
       </c>
     </row>
-    <row r="314" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>6</v>
       </c>
@@ -18271,7 +18265,7 @@
         <v>9</v>
       </c>
       <c r="E314" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F314" t="s">
         <v>11</v>
@@ -18307,7 +18301,7 @@
         <v>68.644626509999995</v>
       </c>
     </row>
-    <row r="315" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>6</v>
       </c>
@@ -18321,7 +18315,7 @@
         <v>9</v>
       </c>
       <c r="E315" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F315" t="s">
         <v>11</v>
@@ -18731,7 +18725,7 @@
         <f>(AA320-AA321)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V320" s="24" t="s">
+      <c r="V320" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W320">
@@ -18821,7 +18815,7 @@
         <f>(AA320-AA321)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V321" s="24" t="s">
+      <c r="V321" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W321">
@@ -19897,7 +19891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>6</v>
       </c>
@@ -19947,7 +19941,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="341" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>6</v>
       </c>
@@ -19997,7 +19991,7 @@
         <v>0.99750000000000005</v>
       </c>
     </row>
-    <row r="342" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>6</v>
       </c>
@@ -20047,7 +20041,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="343" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>6</v>
       </c>
@@ -20097,7 +20091,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="344" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>6</v>
       </c>
@@ -20147,7 +20141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>6</v>
       </c>
@@ -20197,7 +20191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>6</v>
       </c>
@@ -20247,7 +20241,7 @@
         <v>101.5727651</v>
       </c>
     </row>
-    <row r="347" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>6</v>
       </c>
@@ -20297,7 +20291,7 @@
         <v>131.27276509999999</v>
       </c>
     </row>
-    <row r="348" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>6</v>
       </c>
@@ -20352,7 +20346,7 @@
         <v>732.09999999999991</v>
       </c>
     </row>
-    <row r="349" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>6</v>
       </c>
@@ -20422,7 +20416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>6</v>
       </c>
@@ -20492,7 +20486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>6</v>
       </c>
@@ -20562,7 +20556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>6</v>
       </c>
@@ -20647,7 +20641,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="353" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>6</v>
       </c>
@@ -20721,7 +20715,7 @@
         <f>(AA353-AA354)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V353" s="24" t="s">
+      <c r="V353" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W353" s="16">
@@ -20740,7 +20734,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="354" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>6</v>
       </c>
@@ -20814,7 +20808,7 @@
         <f>(AA353-AA354)*(1-$V1)</f>
         <v>52.751999999999995</v>
       </c>
-      <c r="V354" s="24" t="s">
+      <c r="V354" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W354" s="16">
@@ -20833,7 +20827,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="355" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>6</v>
       </c>
@@ -20903,7 +20897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>6</v>
       </c>
@@ -20973,7 +20967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>6</v>
       </c>
@@ -21043,7 +21037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>6</v>
       </c>
@@ -21113,7 +21107,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="359" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>6</v>
       </c>
@@ -21183,7 +21177,7 @@
         <v>269.2</v>
       </c>
     </row>
-    <row r="360" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>6</v>
       </c>
@@ -21253,7 +21247,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="361" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>6</v>
       </c>
@@ -21323,7 +21317,7 @@
         <v>223.5</v>
       </c>
     </row>
-    <row r="362" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>6</v>
       </c>
@@ -21393,7 +21387,7 @@
         <v>153.5</v>
       </c>
     </row>
-    <row r="363" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>6</v>
       </c>
@@ -21443,7 +21437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="364" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>6</v>
       </c>
@@ -21493,7 +21487,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="365" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>6</v>
       </c>
@@ -21543,7 +21537,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="366" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>6</v>
       </c>
@@ -21593,7 +21587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>6</v>
       </c>
@@ -21643,7 +21637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:27" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>6</v>
       </c>
@@ -21693,7 +21687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>6</v>
       </c>
@@ -21706,7 +21700,7 @@
       <c r="D369" t="s">
         <v>9</v>
       </c>
-      <c r="E369" s="26" t="s">
+      <c r="E369" s="24" t="s">
         <v>42</v>
       </c>
       <c r="F369" t="s">
@@ -21743,7 +21737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="370" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>6</v>
       </c>
@@ -21756,7 +21750,7 @@
       <c r="D370" t="s">
         <v>9</v>
       </c>
-      <c r="E370" s="26" t="s">
+      <c r="E370" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F370" t="s">
@@ -21793,7 +21787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>6</v>
       </c>
@@ -21806,7 +21800,7 @@
       <c r="D371" t="s">
         <v>9</v>
       </c>
-      <c r="E371" s="26" t="s">
+      <c r="E371" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F371" t="s">
@@ -21843,7 +21837,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="372" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>6</v>
       </c>
@@ -21856,7 +21850,7 @@
       <c r="D372" t="s">
         <v>9</v>
       </c>
-      <c r="E372" s="26" t="s">
+      <c r="E372" s="24" t="s">
         <v>45</v>
       </c>
       <c r="F372" t="s">
@@ -22627,7 +22621,7 @@
       <c r="U385">
         <v>1.8</v>
       </c>
-      <c r="W385" s="21">
+      <c r="W385" s="20">
         <v>2019</v>
       </c>
       <c r="X385" s="14">
@@ -22717,7 +22711,7 @@
         <f>(AA386-AA387)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V386" s="24" t="s">
+      <c r="V386" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W386" s="16">
@@ -22810,7 +22804,7 @@
         <f>(AA386-AA387)*(1-$V1)</f>
         <v>52.751999999999995</v>
       </c>
-      <c r="V387" s="24" t="s">
+      <c r="V387" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W387" s="16">
@@ -24623,7 +24617,7 @@
       <c r="U418">
         <v>1.8</v>
       </c>
-      <c r="W418" s="21">
+      <c r="W418" s="20">
         <v>2019</v>
       </c>
       <c r="X418" s="14">
@@ -24713,7 +24707,7 @@
         <f>(AA419-AA420)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V419" s="24" t="s">
+      <c r="V419" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W419" s="16">
@@ -24806,7 +24800,7 @@
         <f>(AA419-AA420)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V420" s="24" t="s">
+      <c r="V420" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W420" s="16">
@@ -26615,7 +26609,7 @@
       <c r="U451">
         <v>1.8</v>
       </c>
-      <c r="W451" s="21">
+      <c r="W451" s="20">
         <v>2019</v>
       </c>
       <c r="X451" s="14">
@@ -26705,7 +26699,7 @@
         <f>(AA452-AA453)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V452" s="24" t="s">
+      <c r="V452" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W452" s="16">
@@ -26798,7 +26792,7 @@
         <f>(AA452-AA453)*(1-$V1)</f>
         <v>52.752000000000002</v>
       </c>
-      <c r="V453" s="24" t="s">
+      <c r="V453" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W453" s="16">
@@ -28611,7 +28605,7 @@
       <c r="U484">
         <v>1.8</v>
       </c>
-      <c r="W484" s="21">
+      <c r="W484" s="20">
         <v>2019</v>
       </c>
       <c r="X484" s="14">
@@ -28701,7 +28695,7 @@
         <f>(AA485-AA486)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V485" s="24" t="s">
+      <c r="V485" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W485" s="16">
@@ -28794,7 +28788,7 @@
         <f>(AA485-AA486)*(1-$V1)</f>
         <v>52.667999999999992</v>
       </c>
-      <c r="V486" s="24" t="s">
+      <c r="V486" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W486" s="16">
@@ -30607,7 +30601,7 @@
       <c r="U517">
         <v>1.8</v>
       </c>
-      <c r="W517" s="21">
+      <c r="W517" s="20">
         <v>2019</v>
       </c>
       <c r="X517" s="14">
@@ -30697,7 +30691,7 @@
         <f>(AA518-AA519)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V518" s="24" t="s">
+      <c r="V518" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W518" s="16">
@@ -30790,7 +30784,7 @@
         <f>(AA518-AA519)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V519" s="24" t="s">
+      <c r="V519" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W519" s="16">
@@ -32603,7 +32597,7 @@
       <c r="U550">
         <v>1.8</v>
       </c>
-      <c r="W550" s="21">
+      <c r="W550" s="20">
         <v>2019</v>
       </c>
       <c r="X550" s="14">
@@ -32693,7 +32687,7 @@
         <f>(AA551-AA552)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V551" s="24" t="s">
+      <c r="V551" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W551" s="16">
@@ -32783,7 +32777,7 @@
         <f>(AA551-AA552)*(1-$V1)</f>
         <v>52.751999999999995</v>
       </c>
-      <c r="V552" s="24" t="s">
+      <c r="V552" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W552" s="16">
@@ -34593,7 +34587,7 @@
       <c r="U583">
         <v>1.8</v>
       </c>
-      <c r="W583" s="21">
+      <c r="W583" s="20">
         <v>2019</v>
       </c>
       <c r="X583" s="14">
@@ -34683,10 +34677,10 @@
         <f>(AA584-AA585)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V584" s="24" t="s">
+      <c r="V584" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="W584" s="22">
+      <c r="W584" s="21">
         <v>59.5</v>
       </c>
       <c r="X584" s="8"/>
@@ -34774,10 +34768,10 @@
         <f>(AA584-AA585)*(1-$V1)</f>
         <v>52.751999999999995</v>
       </c>
-      <c r="V585" s="24" t="s">
+      <c r="V585" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="W585" s="23">
+      <c r="W585" s="22">
         <v>5.5</v>
       </c>
       <c r="X585" s="10"/>
@@ -36585,7 +36579,7 @@
       <c r="U616">
         <v>1.8</v>
       </c>
-      <c r="W616" s="21">
+      <c r="W616" s="20">
         <v>2019</v>
       </c>
       <c r="X616" s="14">
@@ -36675,7 +36669,7 @@
         <f>(AA617-AA618)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V617" s="24" t="s">
+      <c r="V617" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W617" s="16">
@@ -36765,7 +36759,7 @@
         <f>(AA617-AA618)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V618" s="24" t="s">
+      <c r="V618" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W618" s="16">
@@ -38575,7 +38569,7 @@
       <c r="U649">
         <v>1.8</v>
       </c>
-      <c r="W649" s="21">
+      <c r="W649" s="20">
         <v>2019</v>
       </c>
       <c r="X649" s="14">
@@ -38665,7 +38659,7 @@
         <f>(AA650-AA651)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V650" s="24" t="s">
+      <c r="V650" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W650" s="16">
@@ -38755,7 +38749,7 @@
         <f>(AA650-AA651)*(1-$V1)</f>
         <v>52.752000000000002</v>
       </c>
-      <c r="V651" s="24" t="s">
+      <c r="V651" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W651" s="16">
@@ -40565,7 +40559,7 @@
       <c r="U682">
         <v>1.8</v>
       </c>
-      <c r="W682" s="21">
+      <c r="W682" s="20">
         <v>2019</v>
       </c>
       <c r="X682" s="14">
@@ -40655,7 +40649,7 @@
         <f>(AA683-AA684)*($V1)</f>
         <v>10.048</v>
       </c>
-      <c r="V683" s="24" t="s">
+      <c r="V683" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W683" s="16">
@@ -40745,7 +40739,7 @@
         <f>(AA683-AA684)*(1-$V1)</f>
         <v>52.751999999999995</v>
       </c>
-      <c r="V684" s="24" t="s">
+      <c r="V684" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W684" s="16">
@@ -42555,7 +42549,7 @@
       <c r="U715">
         <v>1.8</v>
       </c>
-      <c r="W715" s="21">
+      <c r="W715" s="20">
         <v>2019</v>
       </c>
       <c r="X715" s="14">
@@ -42645,7 +42639,7 @@
         <f>(AA716-AA717)*($V1)</f>
         <v>10.032</v>
       </c>
-      <c r="V716" s="24" t="s">
+      <c r="V716" s="23" t="s">
         <v>109</v>
       </c>
       <c r="W716" s="16">
@@ -42735,7 +42729,7 @@
         <f>(AA716-AA717)*(1-$V1)</f>
         <v>52.667999999999999</v>
       </c>
-      <c r="V717" s="24" t="s">
+      <c r="V717" s="23" t="s">
         <v>108</v>
       </c>
       <c r="W717" s="16">
@@ -44111,7 +44105,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="742" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="742" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A742" t="s">
         <v>6</v>
       </c>
@@ -45011,7 +45005,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="760" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="760" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A760" t="s">
         <v>6</v>
       </c>
@@ -45911,7 +45905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="778" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="778" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A778" t="s">
         <v>6</v>
       </c>
@@ -46811,7 +46805,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="796" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="796" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A796" t="s">
         <v>6</v>
       </c>
@@ -47711,7 +47705,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="814" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="814" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A814" t="s">
         <v>6</v>
       </c>
@@ -48611,7 +48605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="832" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="832" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A832" t="s">
         <v>6</v>
       </c>
@@ -49511,7 +49505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="850" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="850" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
         <v>6</v>
       </c>
@@ -53611,7 +53605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="932" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="932" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A932" t="s">
         <v>6</v>
       </c>
@@ -53661,7 +53655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="933" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="933" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A933" t="s">
         <v>6</v>
       </c>
@@ -53711,7 +53705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="934" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="934" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A934" t="s">
         <v>6</v>
       </c>
@@ -53761,7 +53755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="935" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="935" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A935" t="s">
         <v>6</v>
       </c>
@@ -53811,7 +53805,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="936" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="936" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A936" t="s">
         <v>6</v>
       </c>
@@ -53861,7 +53855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="937" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="937" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A937" t="s">
         <v>6</v>
       </c>
@@ -53911,7 +53905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="938" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="938" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A938" t="s">
         <v>6</v>
       </c>
@@ -53961,7 +53955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="939" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="939" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A939" t="s">
         <v>6</v>
       </c>
@@ -54011,7 +54005,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="940" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="940" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A940" t="s">
         <v>6</v>
       </c>
@@ -54061,7 +54055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="941" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="941" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A941" t="s">
         <v>6</v>
       </c>
@@ -54111,7 +54105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="942" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="942" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A942" t="s">
         <v>6</v>
       </c>
@@ -54161,7 +54155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="943" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="943" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A943" t="s">
         <v>6</v>
       </c>
@@ -54211,7 +54205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="944" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="944" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A944" t="s">
         <v>6</v>
       </c>
@@ -54261,7 +54255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="945" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="945" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A945" t="s">
         <v>6</v>
       </c>
@@ -54311,7 +54305,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="946" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="946" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A946" t="s">
         <v>6</v>
       </c>
@@ -54361,7 +54355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="947" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="947" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A947" t="s">
         <v>6</v>
       </c>
@@ -54411,7 +54405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="948" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="948" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A948" t="s">
         <v>6</v>
       </c>
@@ -54461,7 +54455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="949" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="949" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A949" t="s">
         <v>6</v>
       </c>
@@ -54511,7 +54505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="950" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="950" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A950" t="s">
         <v>6</v>
       </c>
@@ -54561,7 +54555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="951" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="951" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A951" t="s">
         <v>6</v>
       </c>
@@ -54611,7 +54605,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="952" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="952" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A952" t="s">
         <v>6</v>
       </c>
@@ -54661,7 +54655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="953" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="953" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A953" t="s">
         <v>6</v>
       </c>
@@ -54711,7 +54705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="954" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="954" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A954" t="s">
         <v>6</v>
       </c>
@@ -54761,7 +54755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="955" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="955" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A955" t="s">
         <v>6</v>
       </c>
@@ -54811,7 +54805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="956" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="956" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A956" t="s">
         <v>6</v>
       </c>
@@ -54861,7 +54855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="957" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="957" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A957" t="s">
         <v>6</v>
       </c>
@@ -54911,7 +54905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="958" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="958" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A958" t="s">
         <v>6</v>
       </c>
@@ -54961,7 +54955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="959" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="959" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A959" t="s">
         <v>6</v>
       </c>
@@ -55011,7 +55005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="960" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="960" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A960" t="s">
         <v>6</v>
       </c>
@@ -55061,7 +55055,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="961" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="961" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A961" t="s">
         <v>6</v>
       </c>
@@ -55111,7 +55105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="962" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="962" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A962" t="s">
         <v>6</v>
       </c>
@@ -55161,7 +55155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="963" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="963" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A963" t="s">
         <v>6</v>
       </c>
@@ -55211,7 +55205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="964" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="964" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A964" t="s">
         <v>6</v>
       </c>
@@ -55261,7 +55255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="965" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="965" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A965" t="s">
         <v>6</v>
       </c>
@@ -55311,7 +55305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="966" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="966" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A966" t="s">
         <v>6</v>
       </c>
@@ -74911,7 +74905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1358" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="1358" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1358" t="s">
         <v>6</v>
       </c>
@@ -75811,7 +75805,7 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="1376" spans="1:21" ht="15" x14ac:dyDescent="0.35">
+    <row r="1376" spans="1:21" ht="15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1376" t="s">
         <v>6</v>
       </c>
@@ -76415,7 +76409,16 @@
   <autoFilter ref="A1:Z1387" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Reference - M0"/>
+        <filter val="Extensive reindustrialization - M0"/>
+        <filter val="Extensive reindustrialization - M1"/>
+        <filter val="Extensive reindustrialization - N2"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Consumption|Electricity|Export"/>
+        <filter val="Production|Electricity|Import"/>
+        <filter val="Production|Electricity|Total without production from flexibility"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>